<commit_message>
Import time-based data to client
</commit_message>
<xml_diff>
--- a/analysis/dashilar.xlsx
+++ b/analysis/dashilar.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="552">
   <si>
     <t>address</t>
   </si>
@@ -745,35 +745,6 @@
   </si>
   <si>
     <t>东城区大栅栏西街56号</t>
-  </si>
-  <si>
-    <t>1 - retail</t>
-  </si>
-  <si>
-    <t>2 - f&amp;b</t>
-  </si>
-  <si>
-    <t>6 - general region (Dashilar, hutongs, etc)</t>
-  </si>
-  <si>
-    <t>0 - outside the region</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>repeats</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>3 - attractions (historic sites, museums)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5 - specific place (bus stop, metro, schools, residential compound etc)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4 - other business (hotel,cinema,banks etc)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>西城区前门西大街正阳市场3号楼</t>
@@ -1815,15 +1786,9 @@
     <t>dianping_tag_2</t>
   </si>
   <si>
-    <t>dianping_addr</t>
-  </si>
-  <si>
     <t>weibo_poiid</t>
   </si>
   <si>
-    <t>weibo_title</t>
-  </si>
-  <si>
     <t>lat_BD</t>
   </si>
   <si>
@@ -1836,9 +1801,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>dianping_title</t>
-  </si>
-  <si>
     <t>北京市 39# Yangmeizhu xiejie-Beijing</t>
   </si>
   <si>
@@ -1849,6 +1811,15 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>alternate title</t>
+  </si>
+  <si>
+    <t>alternate address</t>
   </si>
 </sst>
 </file>
@@ -1904,24 +1875,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2168,12 +2127,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2706,10 +2663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V188"/>
+  <dimension ref="A1:V193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -2735,37 +2692,37 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>554</v>
+        <v>544</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>559</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>550</v>
-      </c>
-      <c r="H1" t="s">
-        <v>555</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J1" t="s">
-        <v>548</v>
+      <c r="J1" s="1" t="s">
+        <v>551</v>
       </c>
       <c r="K1" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="L1" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>1</v>
@@ -2780,19 +2737,19 @@
         <v>4</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>551</v>
+        <v>541</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>552</v>
+        <v>542</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="U1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
     </row>
     <row r="2" spans="1:22">
@@ -2812,7 +2769,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>6</v>
@@ -2854,7 +2811,7 @@
         <v>4</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
@@ -2893,7 +2850,7 @@
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>10</v>
@@ -2929,7 +2886,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>13</v>
@@ -2968,7 +2925,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
@@ -3043,7 +3000,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>19</v>
@@ -3118,7 +3075,7 @@
         <v>2</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>23</v>
@@ -3160,10 +3117,10 @@
         <v>2</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="N11" s="1">
         <v>39.899700000000003</v>
@@ -3202,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>26</v>
@@ -3244,7 +3201,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>28</v>
@@ -3286,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>30</v>
@@ -3328,7 +3285,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>32</v>
@@ -3367,7 +3324,7 @@
         <v>5</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>34</v>
@@ -3403,7 +3360,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>36</v>
@@ -3442,7 +3399,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>38</v>
@@ -3523,7 +3480,7 @@
         <v>2</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>43</v>
@@ -3631,7 +3588,7 @@
         <v>5</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>50</v>
@@ -3880,7 +3837,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>67</v>
@@ -3922,7 +3879,7 @@
         <v>4</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>69</v>
@@ -3964,7 +3921,7 @@
         <v>2</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>71</v>
@@ -4003,7 +3960,7 @@
         <v>2</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>73</v>
@@ -4051,19 +4008,19 @@
         <v>75</v>
       </c>
       <c r="H34" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="J34" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="K34" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="L34" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N34" s="1">
         <v>39.895980000000002</v>
@@ -4102,7 +4059,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>77</v>
@@ -4144,10 +4101,10 @@
         <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="H36" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>79</v>
@@ -4156,10 +4113,10 @@
         <v>79</v>
       </c>
       <c r="K36" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="L36" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N36" s="1">
         <v>39.89528</v>
@@ -4198,7 +4155,7 @@
         <v>4</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>81</v>
@@ -4240,22 +4197,22 @@
         <v>4</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="H38" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>84</v>
       </c>
       <c r="J38" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="K38" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="L38" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N38" s="1">
         <v>39.895589999999899</v>
@@ -4294,7 +4251,7 @@
         <v>4</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>86</v>
@@ -4372,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>91</v>
@@ -4570,7 +4527,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>105</v>
@@ -4609,7 +4566,7 @@
         <v>4</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>107</v>
@@ -4720,22 +4677,22 @@
         <v>2</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H50" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>115</v>
       </c>
       <c r="J50" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="K50" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="L50" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="N50" s="1">
         <v>39.894779999999898</v>
@@ -4774,7 +4731,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>117</v>
@@ -4858,7 +4815,7 @@
         <v>2</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>122</v>
@@ -4900,22 +4857,22 @@
         <v>4</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="H54" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>124</v>
       </c>
       <c r="J54" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="K54" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L54" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="N54" s="1">
         <v>39.893300000000004</v>
@@ -4951,7 +4908,7 @@
         <v>1</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>126</v>
@@ -4990,22 +4947,22 @@
         <v>2</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H56" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>128</v>
       </c>
       <c r="J56" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="K56" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="L56" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N56" s="1">
         <v>39.894880000000001</v>
@@ -5041,7 +4998,7 @@
         <v>2</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>130</v>
@@ -5077,7 +5034,7 @@
         <v>5</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="N58" s="1">
         <v>39.893889999999899</v>
@@ -5116,7 +5073,7 @@
         <v>4</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>133</v>
@@ -5158,22 +5115,22 @@
         <v>4</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="H60" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>135</v>
       </c>
       <c r="J60" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="K60" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L60" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="N60" s="1">
         <v>39.894880000000001</v>
@@ -5212,7 +5169,7 @@
         <v>3</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>138</v>
@@ -5254,7 +5211,7 @@
         <v>2</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="I62" s="1" t="s">
         <v>140</v>
@@ -5293,7 +5250,7 @@
         <v>6</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="I63" s="1" t="s">
         <v>142</v>
@@ -5332,22 +5289,22 @@
         <v>2</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="H64" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>144</v>
       </c>
       <c r="J64" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="K64" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L64" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N64" s="1">
         <v>39.894877352999899</v>
@@ -5386,22 +5343,22 @@
         <v>2</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="H65" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>146</v>
       </c>
       <c r="J65" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="K65" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="L65" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N65" s="1">
         <v>39.895150000000001</v>
@@ -5440,22 +5397,22 @@
         <v>2</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H66" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>148</v>
       </c>
       <c r="J66" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="K66" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="L66" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N66" s="1">
         <v>39.894770000000001</v>
@@ -5497,7 +5454,7 @@
         <v>4</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>150</v>
@@ -5539,10 +5496,10 @@
         <v>2</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="H68" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>152</v>
@@ -5551,10 +5508,10 @@
         <v>152</v>
       </c>
       <c r="K68" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="L68" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N68" s="1">
         <v>39.895400000000002</v>
@@ -5593,22 +5550,22 @@
         <v>2</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="H69" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>154</v>
       </c>
       <c r="J69" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="K69" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="L69" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="M69" s="2">
         <v>72</v>
@@ -5650,22 +5607,22 @@
         <v>4</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="H70" s="10" t="s">
-        <v>393</v>
+        <v>303</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>385</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="J70" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="K70" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="L70" s="10" t="s">
-        <v>356</v>
+      <c r="J70" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="K70" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="L70" s="8" t="s">
+        <v>348</v>
       </c>
       <c r="N70" s="1">
         <v>39.894989000000002</v>
@@ -5682,7 +5639,7 @@
       <c r="T70" s="1">
         <v>162</v>
       </c>
-      <c r="U70" s="10">
+      <c r="U70" s="8">
         <v>59</v>
       </c>
       <c r="V70" s="1">
@@ -5704,7 +5661,7 @@
         <v>2</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>158</v>
@@ -5779,7 +5736,7 @@
         <v>4</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>163</v>
@@ -5821,7 +5778,7 @@
         <v>2</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>165</v>
@@ -5863,7 +5820,7 @@
         <v>4</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>167</v>
@@ -5905,7 +5862,7 @@
         <v>2</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>169</v>
@@ -5944,7 +5901,7 @@
         <v>2</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>171</v>
@@ -6019,7 +5976,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>176</v>
@@ -6061,7 +6018,7 @@
         <v>4</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>178</v>
@@ -6139,7 +6096,7 @@
         <v>4</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>183</v>
@@ -6181,7 +6138,7 @@
         <v>2</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>185</v>
@@ -6220,7 +6177,7 @@
         <v>2</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>187</v>
@@ -6262,7 +6219,7 @@
         <v>3</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>189</v>
@@ -6376,7 +6333,7 @@
         <v>2</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>198</v>
@@ -6418,7 +6375,7 @@
         <v>4</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>200</v>
@@ -6463,7 +6420,7 @@
         <v>2</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>202</v>
@@ -6505,7 +6462,7 @@
         <v>4</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>204</v>
@@ -6547,7 +6504,7 @@
         <v>2</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>207</v>
@@ -6622,7 +6579,7 @@
         <v>4</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>211</v>
@@ -6664,10 +6621,10 @@
         <v>2</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="N95" s="1">
         <v>39.899794132731003</v>
@@ -6706,22 +6663,22 @@
         <v>2</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="H96" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>214</v>
       </c>
       <c r="J96" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="K96" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="L96" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N96" s="1">
         <v>39.899464000000002</v>
@@ -6760,7 +6717,7 @@
         <v>2</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>216</v>
@@ -6802,22 +6759,22 @@
         <v>2</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="H98" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>219</v>
       </c>
       <c r="J98" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="K98" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="L98" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N98" s="1">
         <v>39.895879999999899</v>
@@ -6856,7 +6813,7 @@
         <v>2</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>221</v>
@@ -6898,22 +6855,22 @@
         <v>2</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="H100" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>223</v>
       </c>
       <c r="J100" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="K100" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="L100" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N100" s="1">
         <v>39.893602000000001</v>
@@ -6952,22 +6909,22 @@
         <v>2</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="H101" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="J101" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="K101" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="L101" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="M101" s="2">
         <v>58</v>
@@ -7009,22 +6966,22 @@
         <v>2</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="H102" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>226</v>
       </c>
       <c r="J102" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="K102" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="L102" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N102" s="1">
         <v>39.893000000000001</v>
@@ -7060,7 +7017,7 @@
         <v>2</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>228</v>
@@ -7099,22 +7056,22 @@
         <v>4</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="H104" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>230</v>
       </c>
       <c r="J104" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="K104" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L104" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N104" s="1">
         <v>39.895235999999898</v>
@@ -7153,22 +7110,22 @@
         <v>4</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H105" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>232</v>
       </c>
       <c r="J105" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="K105" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L105" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="N105" s="1">
         <v>39.894849999999899</v>
@@ -7203,13 +7160,13 @@
       <c r="F106" s="1">
         <v>1</v>
       </c>
-      <c r="G106" s="9" t="s">
-        <v>340</v>
-      </c>
-      <c r="I106" s="7" t="s">
-        <v>252</v>
-      </c>
-      <c r="M106" s="6">
+      <c r="G106" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="M106" s="4">
         <v>68</v>
       </c>
       <c r="P106" s="1">
@@ -7242,13 +7199,13 @@
       <c r="F107" s="1">
         <v>1</v>
       </c>
-      <c r="G107" s="5" t="s">
-        <v>341</v>
-      </c>
-      <c r="I107" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="M107" s="7">
+      <c r="G107" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="I107" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="M107" s="5">
         <v>29</v>
       </c>
       <c r="P107" s="1">
@@ -7281,13 +7238,13 @@
       <c r="F108" s="1">
         <v>1</v>
       </c>
-      <c r="G108" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="I108" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="M108" s="7">
+      <c r="G108" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="M108" s="5">
         <v>69</v>
       </c>
       <c r="P108" s="1">
@@ -7320,25 +7277,25 @@
       <c r="F109" s="1">
         <v>1</v>
       </c>
-      <c r="G109" s="8" t="s">
-        <v>343</v>
+      <c r="G109" s="6" t="s">
+        <v>335</v>
       </c>
       <c r="H109" t="s">
-        <v>372</v>
-      </c>
-      <c r="I109" s="7" t="s">
-        <v>247</v>
+        <v>364</v>
+      </c>
+      <c r="I109" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="J109" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="K109" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="L109" t="s">
-        <v>356</v>
-      </c>
-      <c r="M109" s="7">
+        <v>348</v>
+      </c>
+      <c r="M109" s="5">
         <v>31</v>
       </c>
       <c r="P109" s="1">
@@ -7371,13 +7328,13 @@
       <c r="F110" s="1">
         <v>1</v>
       </c>
-      <c r="G110" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="I110" s="7" t="s">
-        <v>248</v>
-      </c>
-      <c r="M110" s="7">
+      <c r="G110" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="I110" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="M110" s="5">
         <v>33</v>
       </c>
       <c r="P110" s="1">
@@ -7410,11 +7367,11 @@
       <c r="F111" s="1">
         <v>1</v>
       </c>
-      <c r="G111" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="I111" s="7" t="s">
-        <v>261</v>
+      <c r="G111" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>253</v>
       </c>
       <c r="P111" s="1">
         <v>39.8946726896</v>
@@ -7446,25 +7403,25 @@
       <c r="F112" s="1">
         <v>1</v>
       </c>
-      <c r="G112" s="5" t="s">
-        <v>346</v>
+      <c r="G112" s="3" t="s">
+        <v>338</v>
       </c>
       <c r="H112" t="s">
-        <v>384</v>
-      </c>
-      <c r="I112" s="7" t="s">
-        <v>254</v>
+        <v>376</v>
+      </c>
+      <c r="I112" s="5" t="s">
+        <v>246</v>
       </c>
       <c r="J112" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="K112" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="L112" t="s">
-        <v>356</v>
-      </c>
-      <c r="M112" s="5">
+        <v>348</v>
+      </c>
+      <c r="M112" s="3">
         <v>70</v>
       </c>
       <c r="P112" s="1">
@@ -7497,25 +7454,25 @@
       <c r="F113" s="1">
         <v>1</v>
       </c>
-      <c r="G113" s="5" t="s">
-        <v>243</v>
+      <c r="G113" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="H113" t="s">
-        <v>354</v>
-      </c>
-      <c r="I113" s="7" t="s">
-        <v>249</v>
+        <v>346</v>
+      </c>
+      <c r="I113" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="J113" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="K113" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="L113" t="s">
-        <v>356</v>
-      </c>
-      <c r="M113" s="7">
+        <v>348</v>
+      </c>
+      <c r="M113" s="5">
         <v>36</v>
       </c>
       <c r="P113" s="1">
@@ -7548,13 +7505,13 @@
       <c r="F114" s="1">
         <v>1</v>
       </c>
-      <c r="G114" s="5" t="s">
-        <v>347</v>
-      </c>
-      <c r="I114" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="M114" s="7">
+      <c r="G114" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="I114" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="M114" s="5">
         <v>38</v>
       </c>
       <c r="P114" s="1">
@@ -7587,23 +7544,23 @@
       <c r="F115" s="1">
         <v>1</v>
       </c>
-      <c r="G115" s="9" t="s">
+      <c r="G115" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="H115" t="s">
+        <v>381</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="J115" t="s">
+        <v>382</v>
+      </c>
+      <c r="K115" t="s">
+        <v>352</v>
+      </c>
+      <c r="L115" t="s">
         <v>348</v>
-      </c>
-      <c r="H115" t="s">
-        <v>389</v>
-      </c>
-      <c r="I115" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="J115" t="s">
-        <v>390</v>
-      </c>
-      <c r="K115" t="s">
-        <v>360</v>
-      </c>
-      <c r="L115" t="s">
-        <v>356</v>
       </c>
       <c r="P115" s="1">
         <v>39.894195431100002</v>
@@ -7635,11 +7592,11 @@
       <c r="F116" s="1">
         <v>1</v>
       </c>
-      <c r="G116" s="9" t="s">
-        <v>349</v>
-      </c>
-      <c r="I116" s="7" t="s">
-        <v>259</v>
+      <c r="G116" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>251</v>
       </c>
       <c r="P116" s="1">
         <v>39.8941620298</v>
@@ -7671,25 +7628,25 @@
       <c r="F117" s="1">
         <v>2</v>
       </c>
-      <c r="G117" s="9" t="s">
-        <v>350</v>
+      <c r="G117" s="7" t="s">
+        <v>342</v>
       </c>
       <c r="H117" t="s">
-        <v>370</v>
-      </c>
-      <c r="I117" s="6" t="s">
-        <v>251</v>
+        <v>362</v>
+      </c>
+      <c r="I117" s="4" t="s">
+        <v>243</v>
       </c>
       <c r="J117" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="K117" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="L117" t="s">
-        <v>356</v>
-      </c>
-      <c r="M117" s="7">
+        <v>348</v>
+      </c>
+      <c r="M117" s="5">
         <v>57</v>
       </c>
       <c r="P117" s="1">
@@ -7722,25 +7679,25 @@
       <c r="F118" s="1">
         <v>2</v>
       </c>
-      <c r="G118" s="5" t="s">
-        <v>244</v>
+      <c r="G118" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="H118" t="s">
-        <v>405</v>
-      </c>
-      <c r="I118" s="6" t="s">
-        <v>255</v>
+        <v>397</v>
+      </c>
+      <c r="I118" s="4" t="s">
+        <v>247</v>
       </c>
       <c r="J118" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="K118" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="L118" t="s">
-        <v>356</v>
-      </c>
-      <c r="M118" s="5">
+        <v>348</v>
+      </c>
+      <c r="M118" s="3">
         <v>71</v>
       </c>
       <c r="P118" s="1">
@@ -7773,13 +7730,13 @@
       <c r="F119" s="1">
         <v>3</v>
       </c>
-      <c r="G119" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="I119" s="8" t="s">
-        <v>256</v>
-      </c>
-      <c r="M119" s="7">
+      <c r="G119" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="M119" s="5">
         <v>74</v>
       </c>
       <c r="P119" s="1">
@@ -7812,13 +7769,13 @@
       <c r="F120" s="1">
         <v>3</v>
       </c>
-      <c r="G120" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="I120" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="M120" s="6">
+      <c r="G120" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="I120" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="M120" s="4">
         <v>75</v>
       </c>
       <c r="P120" s="1">
@@ -7851,25 +7808,25 @@
       <c r="F121" s="1">
         <v>2</v>
       </c>
-      <c r="G121" s="9" t="s">
+      <c r="G121" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H121" t="s">
+        <v>373</v>
+      </c>
+      <c r="I121" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="J121" t="s">
+        <v>374</v>
+      </c>
+      <c r="K121" t="s">
         <v>352</v>
       </c>
-      <c r="H121" t="s">
-        <v>381</v>
-      </c>
-      <c r="I121" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="J121" t="s">
-        <v>382</v>
-      </c>
-      <c r="K121" t="s">
-        <v>360</v>
-      </c>
       <c r="L121" t="s">
-        <v>356</v>
-      </c>
-      <c r="M121" s="9">
+        <v>348</v>
+      </c>
+      <c r="M121" s="7">
         <v>78</v>
       </c>
       <c r="P121" s="1">
@@ -7903,16 +7860,16 @@
         <v>2</v>
       </c>
       <c r="G122" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="J122" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="K122" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L122" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P122" s="1">
         <v>39.893032070300002</v>
@@ -7945,16 +7902,16 @@
         <v>1</v>
       </c>
       <c r="G123" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="J123" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="K123" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="L123" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P123" s="1">
         <v>39.894226721800003</v>
@@ -7987,16 +7944,16 @@
         <v>2</v>
       </c>
       <c r="G124" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="J124" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="K124" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="L124" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P124" s="1">
         <v>39.893464437299997</v>
@@ -8029,16 +7986,16 @@
         <v>1</v>
       </c>
       <c r="G125" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="J125" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="K125" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="L125" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P125" s="1">
         <v>39.8935794012</v>
@@ -8071,16 +8028,16 @@
         <v>2</v>
       </c>
       <c r="G126" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="J126" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="K126" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L126" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P126" s="1">
         <v>39.893294845100002</v>
@@ -8113,16 +8070,16 @@
         <v>4</v>
       </c>
       <c r="G127" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="J127" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="K127" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="L127" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P127" s="1">
         <v>39.893578383600001</v>
@@ -8155,16 +8112,16 @@
         <v>1</v>
       </c>
       <c r="G128" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="J128" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="K128" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="L128" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P128" s="1">
         <v>39.8935811168</v>
@@ -8197,16 +8154,16 @@
         <v>4</v>
       </c>
       <c r="G129" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="J129" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="K129" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L129" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P129" s="1">
         <v>39.893112525200003</v>
@@ -8239,16 +8196,16 @@
         <v>2</v>
       </c>
       <c r="G130" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="J130" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="K130" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L130" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P130" s="1">
         <v>39.8931789978</v>
@@ -8281,16 +8238,16 @@
         <v>2</v>
       </c>
       <c r="G131" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="J131" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="K131" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L131" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P131" s="1">
         <v>39.894112652300002</v>
@@ -8323,16 +8280,16 @@
         <v>4</v>
       </c>
       <c r="G132" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="J132" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="K132" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L132" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P132" s="1">
         <v>39.894253292599998</v>
@@ -8365,16 +8322,16 @@
         <v>2</v>
       </c>
       <c r="G133" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="J133" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="K133" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L133" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="P133" s="1">
         <v>39.891242753900002</v>
@@ -8407,16 +8364,16 @@
         <v>2</v>
       </c>
       <c r="G134" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="J134" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="K134" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="L134" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P134" s="1">
         <v>39.8935809285</v>
@@ -8449,16 +8406,16 @@
         <v>2</v>
       </c>
       <c r="G135" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="J135" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="K135" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="L135" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P135" s="1">
         <v>39.893221264200001</v>
@@ -8491,16 +8448,16 @@
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="J136" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="K136" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="L136" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P136" s="1">
         <v>39.893292825400003</v>
@@ -8533,16 +8490,16 @@
         <v>4</v>
       </c>
       <c r="G137" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="J137" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="K137" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L137" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P137" s="1">
         <v>39.893863613800001</v>
@@ -8575,16 +8532,16 @@
         <v>2</v>
       </c>
       <c r="G138" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="J138" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="K138" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="L138" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="P138" s="1">
         <v>39.892277239599998</v>
@@ -8617,16 +8574,16 @@
         <v>2</v>
       </c>
       <c r="G139" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="J139" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="K139" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="L139" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P139" s="1">
         <v>39.894313863199997</v>
@@ -8659,16 +8616,16 @@
         <v>4</v>
       </c>
       <c r="G140" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="J140" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="K140" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L140" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P140" s="1">
         <v>39.889885337999999</v>
@@ -8701,16 +8658,16 @@
         <v>4</v>
       </c>
       <c r="G141" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="J141" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="K141" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L141" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P141" s="1">
         <v>39.892982096600001</v>
@@ -8745,17 +8702,17 @@
       <c r="F142" s="2">
         <v>2</v>
       </c>
-      <c r="G142" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="J142" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="K142" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="L142" s="10" t="s">
-        <v>466</v>
+      <c r="G142" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="J142" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="K142" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="L142" s="8" t="s">
+        <v>458</v>
       </c>
       <c r="P142" s="1">
         <v>39.896889379800001</v>
@@ -8769,7 +8726,7 @@
       <c r="S142" s="2">
         <v>116.395556</v>
       </c>
-      <c r="U142" s="10">
+      <c r="U142" s="8">
         <v>2</v>
       </c>
       <c r="V142" s="1">
@@ -8788,16 +8745,16 @@
         <v>2</v>
       </c>
       <c r="G143" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="J143" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="K143" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="L143" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P143" s="1">
         <v>39.8943831944</v>
@@ -8830,16 +8787,16 @@
         <v>2</v>
       </c>
       <c r="G144" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="J144" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="K144" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="L144" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="P144" s="1">
         <v>39.892969729000001</v>
@@ -8872,16 +8829,16 @@
         <v>2</v>
       </c>
       <c r="G145" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="J145" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="K145" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="L145" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P145" s="1">
         <v>39.893156874500001</v>
@@ -8914,16 +8871,16 @@
         <v>2</v>
       </c>
       <c r="G146" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="J146" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="K146" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L146" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P146" s="1">
         <v>39.890443335400001</v>
@@ -8956,16 +8913,16 @@
         <v>4</v>
       </c>
       <c r="G147" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="J147" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="K147" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="L147" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P147" s="1">
         <v>39.893343009200002</v>
@@ -8998,16 +8955,16 @@
         <v>2</v>
       </c>
       <c r="G148" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="J148" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="K148" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="L148" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P148" s="1">
         <v>39.892350886099997</v>
@@ -9040,16 +8997,16 @@
         <v>2</v>
       </c>
       <c r="G149" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="J149" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="K149" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="L149" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P149" s="1">
         <v>39.893156874500001</v>
@@ -9082,16 +9039,16 @@
         <v>2</v>
       </c>
       <c r="G150" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="J150" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="K150" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L150" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P150" s="1">
         <v>39.894997846300001</v>
@@ -9124,16 +9081,16 @@
         <v>4</v>
       </c>
       <c r="G151" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="J151" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="K151" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="L151" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P151" s="1">
         <v>39.893743147599999</v>
@@ -9166,16 +9123,16 @@
         <v>4</v>
       </c>
       <c r="G152" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="J152" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="K152" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L152" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P152" s="1">
         <v>39.8927354327</v>
@@ -9208,16 +9165,16 @@
         <v>1</v>
       </c>
       <c r="G153" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="J153" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="K153" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="L153" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P153" s="1">
         <v>39.894308641099997</v>
@@ -9250,16 +9207,16 @@
         <v>2</v>
       </c>
       <c r="G154" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="J154" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="K154" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="L154" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="P154" s="1">
         <v>39.888831453000002</v>
@@ -9292,13 +9249,13 @@
         <v>2</v>
       </c>
       <c r="G155" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="J155" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="K155" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="L155"/>
       <c r="P155" s="1">
@@ -9332,16 +9289,16 @@
         <v>2</v>
       </c>
       <c r="G156" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="J156" t="s">
         <v>152</v>
       </c>
       <c r="K156" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L156" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P156" s="1">
         <v>39.892929834299999</v>
@@ -9374,16 +9331,16 @@
         <v>4</v>
       </c>
       <c r="G157" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="J157" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="K157" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L157" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P157" s="1">
         <v>39.892428750599997</v>
@@ -9416,16 +9373,16 @@
         <v>4</v>
       </c>
       <c r="G158" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="J158" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="K158" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="L158" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P158" s="1">
         <v>39.893976842199997</v>
@@ -9458,16 +9415,16 @@
         <v>4</v>
       </c>
       <c r="G159" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="J159" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="K159" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L159" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P159" s="1">
         <v>39.892925015199999</v>
@@ -9500,16 +9457,16 @@
         <v>4</v>
       </c>
       <c r="G160" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="J160" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="K160" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="L160" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="P160" s="1">
         <v>39.894362530999999</v>
@@ -9542,16 +9499,16 @@
         <v>2</v>
       </c>
       <c r="G161" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="J161" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="K161" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L161" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P161" s="1">
         <v>39.892804230800003</v>
@@ -9584,16 +9541,16 @@
         <v>4</v>
       </c>
       <c r="G162" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="J162" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="K162" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L162" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P162" s="1">
         <v>39.8937491493</v>
@@ -9626,16 +9583,16 @@
         <v>1</v>
       </c>
       <c r="G163" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="J163" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="K163" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="L163" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P163" s="1">
         <v>39.8943083415</v>
@@ -9668,16 +9625,16 @@
         <v>2</v>
       </c>
       <c r="G164" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="J164" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="K164" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="L164" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="P164" s="1">
         <v>39.893083086300003</v>
@@ -9710,16 +9667,16 @@
         <v>4</v>
       </c>
       <c r="G165" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="J165" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="K165" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="L165" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P165" s="1">
         <v>39.893328499100001</v>
@@ -9752,16 +9709,16 @@
         <v>4</v>
       </c>
       <c r="G166" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="J166" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="K166" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L166" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P166" s="1">
         <v>39.892339518299998</v>
@@ -9794,16 +9751,16 @@
         <v>1</v>
       </c>
       <c r="G167" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="J167" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="K167" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="L167" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P167" s="1">
         <v>39.894077144100002</v>
@@ -9836,16 +9793,16 @@
         <v>4</v>
       </c>
       <c r="G168" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="J168" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="K168" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="L168" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="P168" s="1">
         <v>39.893235112900001</v>
@@ -9878,16 +9835,16 @@
         <v>2</v>
       </c>
       <c r="G169" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="J169" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="K169" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="L169" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P169" s="1">
         <v>39.894056599199999</v>
@@ -9920,16 +9877,16 @@
         <v>1</v>
       </c>
       <c r="G170" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="J170" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="K170" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="L170" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="P170" s="1">
         <v>39.894501620699998</v>
@@ -9962,16 +9919,16 @@
         <v>4</v>
       </c>
       <c r="G171" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="J171" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="K171" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="L171" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P171" s="1">
         <v>39.894003314099997</v>
@@ -10004,16 +9961,16 @@
         <v>2</v>
       </c>
       <c r="G172" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="J172" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="K172" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="L172" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P172" s="1">
         <v>39.8930928905</v>
@@ -10046,16 +10003,16 @@
         <v>2</v>
       </c>
       <c r="G173" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="J173" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="K173" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="L173" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P173" s="1">
         <v>39.893032070300002</v>
@@ -10088,16 +10045,16 @@
         <v>2</v>
       </c>
       <c r="G174" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="J174" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="K174" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="L174" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P174" s="1">
         <v>39.893912351899999</v>
@@ -10130,16 +10087,16 @@
         <v>2</v>
       </c>
       <c r="G175" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="J175" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="K175" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="L175" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P175" s="1">
         <v>39.8943831944</v>
@@ -10172,16 +10129,16 @@
         <v>4</v>
       </c>
       <c r="G176" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="J176" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="K176" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="L176" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="P176" s="1">
         <v>39.890979048799998</v>
@@ -10214,16 +10171,16 @@
         <v>4</v>
       </c>
       <c r="G177" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="J177" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="K177" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="L177" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="P177" s="1">
         <v>39.896607996199997</v>
@@ -10245,45 +10202,41 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="1:22">
-      <c r="A181" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
     <row r="182" spans="1:22">
-      <c r="A182" s="1" t="s">
-        <v>234</v>
-      </c>
+      <c r="A182" s="2"/>
     </row>
     <row r="183" spans="1:22">
-      <c r="A183" s="1" t="s">
-        <v>238</v>
-      </c>
+      <c r="A183" s="2"/>
     </row>
     <row r="184" spans="1:22">
-      <c r="A184" s="1" t="s">
-        <v>240</v>
-      </c>
+      <c r="A184" s="2"/>
     </row>
     <row r="185" spans="1:22">
-      <c r="A185" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="A185" s="2"/>
     </row>
     <row r="186" spans="1:22">
-      <c r="A186" s="1" t="s">
-        <v>235</v>
-      </c>
+      <c r="A186" s="2"/>
     </row>
     <row r="187" spans="1:22">
-      <c r="A187" s="3" t="s">
-        <v>236</v>
-      </c>
+      <c r="A187" s="2"/>
     </row>
     <row r="188" spans="1:22">
-      <c r="A188" s="4" t="s">
-        <v>237</v>
-      </c>
+      <c r="A188" s="2"/>
+    </row>
+    <row r="189" spans="1:22">
+      <c r="A189" s="2"/>
+    </row>
+    <row r="190" spans="1:22">
+      <c r="A190" s="2"/>
+    </row>
+    <row r="191" spans="1:22">
+      <c r="A191" s="2"/>
+    </row>
+    <row r="192" spans="1:22">
+      <c r="A192" s="2"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>